<commit_message>
last hurrah of trying variability analysis
</commit_message>
<xml_diff>
--- a/input/FUCCI staining review_variation_annotation_EL.xlsx
+++ b/input/FUCCI staining review_variation_annotation_EL.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antho\Documents\Projects\CellCycle\FucciRNA\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{664F7BCA-02DF-4898-ABC4-18BCA6D8FCD8}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED24D251-2645-4483-A332-D3D79F5D036B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="52930" yWindow="5780" windowWidth="21600" windowHeight="11260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1990" yWindow="3980" windowWidth="21620" windowHeight="11280" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="6717" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3126" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3127" uniqueCount="223">
   <si>
     <t>Well</t>
   </si>
@@ -1038,8 +1038,8 @@
   </sheetPr>
   <dimension ref="A1:L97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1845,6 +1845,9 @@
       </c>
       <c r="H28" s="3">
         <v>1</v>
+      </c>
+      <c r="I28" t="s">
+        <v>18</v>
       </c>
       <c r="K28" s="3" t="s">
         <v>27</v>
@@ -3837,8 +3840,8 @@
   </sheetPr>
   <dimension ref="A1:L97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="K95" sqref="K95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -6535,8 +6538,8 @@
   </sheetPr>
   <dimension ref="A1:L97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="K97" sqref="K97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -9248,7 +9251,7 @@
   </sheetPr>
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A51" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -15964,8 +15967,8 @@
   </sheetPr>
   <dimension ref="A1:L97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="K95" sqref="K95:K96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -18741,7 +18744,7 @@
   <dimension ref="A1:L97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -18865,7 +18868,10 @@
       <c r="H4" s="3">
         <v>0</v>
       </c>
-      <c r="L4" s="2"/>
+      <c r="L4" s="2">
+        <f>SUMIF(K:K,"Unspecific",C:H)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:12" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
@@ -21463,7 +21469,7 @@
   <dimension ref="A1:L97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -21563,7 +21569,10 @@
       <c r="H3" s="3">
         <v>0</v>
       </c>
-      <c r="L3" s="2"/>
+      <c r="L3" s="2">
+        <f>SUMIF(K:K,"Unspecific",C:H)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:12" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
@@ -24194,10 +24203,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:J1000"/>
+  <dimension ref="A1:K1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -24205,7 +24214,7 @@
     <col min="1" max="26" width="10.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -24234,7 +24243,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -24258,7 +24267,7 @@
         <v>B12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>
@@ -24282,8 +24291,9 @@
         <f t="shared" ref="J3:J66" si="0">LEFT(A3)&amp;IF(LEN(A3)=2,"0","")&amp;RIGHT(A3,LEN(A3)-1)</f>
         <v>B11</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -24307,7 +24317,7 @@
         <v>B10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>96</v>
       </c>
@@ -24338,7 +24348,7 @@
         <v>B09</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>95</v>
       </c>
@@ -24365,7 +24375,7 @@
         <v>B08</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>94</v>
       </c>
@@ -24393,7 +24403,7 @@
         <v>B07</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>93</v>
       </c>
@@ -24417,7 +24427,7 @@
         <v>B06</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>91</v>
       </c>
@@ -24441,7 +24451,7 @@
         <v>B05</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>89</v>
       </c>
@@ -24465,7 +24475,7 @@
         <v>B04</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>87</v>
       </c>
@@ -24489,7 +24499,7 @@
         <v>B03</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>84</v>
       </c>
@@ -24516,7 +24526,7 @@
         <v>B02</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>83</v>
       </c>
@@ -24540,7 +24550,7 @@
         <v>B01</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>11</v>
       </c>
@@ -24565,7 +24575,7 @@
         <v>A12</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -24590,7 +24600,7 @@
         <v>A11</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -25462,16 +25472,16 @@
         <v>12</v>
       </c>
       <c r="C49" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D49" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E49" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F49" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>55</v>
@@ -27623,10 +27633,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L97"/>
+  <dimension ref="A1:M97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A97"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -27636,7 +27646,7 @@
     <col min="3" max="8" width="4.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -27671,7 +27681,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -27703,8 +27713,12 @@
         <f>LEFT(A2)&amp;IF(LEN(A2)=2,"0","")&amp;RIGHT(A2,LEN(A2)-1)</f>
         <v>A12</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="12.75" x14ac:dyDescent="0.35">
+      <c r="M2">
+        <f>SUMIF(K:K,"Unspecific",C:H)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -27734,7 +27748,7 @@
         <v>A11</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -27767,7 +27781,7 @@
         <v>A10</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>78</v>
       </c>
@@ -27797,7 +27811,7 @@
         <v>A09</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>76</v>
       </c>
@@ -27827,7 +27841,7 @@
         <v>A08</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>75</v>
       </c>
@@ -27860,7 +27874,7 @@
         <v>A07</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>73</v>
       </c>
@@ -27893,7 +27907,7 @@
         <v>A06</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>71</v>
       </c>
@@ -27923,7 +27937,7 @@
         <v>A05</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>70</v>
       </c>
@@ -27956,7 +27970,7 @@
         <v>A04</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>69</v>
       </c>
@@ -27986,7 +28000,7 @@
         <v>A03</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>68</v>
       </c>
@@ -28019,7 +28033,7 @@
         <v>A02</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>66</v>
       </c>
@@ -28052,7 +28066,7 @@
         <v>A01</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
@@ -28082,7 +28096,7 @@
         <v>B12</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -28118,7 +28132,7 @@
         <v>B11</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="12.75" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>22</v>
       </c>
@@ -30662,8 +30676,8 @@
   </sheetPr>
   <dimension ref="A1:L97"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L2" sqref="L1:L1048576"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -31559,7 +31573,7 @@
         <v>16</v>
       </c>
       <c r="C32" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D32" s="3">
         <v>1</v>
@@ -33399,8 +33413,8 @@
   </sheetPr>
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -35113,10 +35127,10 @@
         <v>85</v>
       </c>
       <c r="C57" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D57" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E57" s="6">
         <v>1</v>
@@ -39022,8 +39036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:L1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="K81" sqref="K81:K82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -42628,8 +42642,8 @@
   </sheetPr>
   <dimension ref="A1:L97"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="K95" sqref="K95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>